<commit_message>
Feb 15th commit #4
</commit_message>
<xml_diff>
--- a/src/main/java/com/jostens/qa/testdata/Jostens.xlsx
+++ b/src/main/java/com/jostens/qa/testdata/Jostens.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="158">
   <si>
     <t>School Name</t>
   </si>
@@ -469,6 +469,36 @@
   </si>
   <si>
     <t>Success - 2021/02/15 20:38:01</t>
+  </si>
+  <si>
+    <t>Success - 2021/02/15 20:47:57</t>
+  </si>
+  <si>
+    <t>Success - 2021/02/15 20:48:00</t>
+  </si>
+  <si>
+    <t>Success - 2021/02/15 20:48:32</t>
+  </si>
+  <si>
+    <t>Success - 2021/02/15 20:49:00</t>
+  </si>
+  <si>
+    <t>Success - 2021/02/15 20:49:27</t>
+  </si>
+  <si>
+    <t>Success - 2021/02/15 20:49:30</t>
+  </si>
+  <si>
+    <t>Success - 2021/02/15 20:49:39</t>
+  </si>
+  <si>
+    <t>Success - 2021/02/15 20:49:50</t>
+  </si>
+  <si>
+    <t>Success - 2021/02/15 20:49:58</t>
+  </si>
+  <si>
+    <t>Success - 2021/02/15 20:50:14</t>
   </si>
 </sst>
 </file>
@@ -829,7 +859,7 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -840,7 +870,7 @@
         <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -899,7 +929,7 @@
         <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1072,7 +1102,7 @@
         <v>115</v>
       </c>
       <c r="G2" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1095,7 +1125,7 @@
         <v>115</v>
       </c>
       <c r="G3" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1118,7 +1148,7 @@
         <v>115</v>
       </c>
       <c r="G4" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1253,7 +1283,7 @@
         <v>42</v>
       </c>
       <c r="P2" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1303,7 +1333,7 @@
         <v>42</v>
       </c>
       <c r="P3" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1353,7 +1383,7 @@
         <v>42</v>
       </c>
       <c r="P4" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1423,7 +1453,7 @@
         <v>92</v>
       </c>
       <c r="F2" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>